<commit_message>
Update check-in functionality and add download button for check-ins
</commit_message>
<xml_diff>
--- a/static/check_ins.xlsx
+++ b/static/check_ins.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,7 +459,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2024-04-11 15:12:18</t>
+          <t>2024-04-11 16:05:28</t>
         </is>
       </c>
     </row>
@@ -472,7 +472,33 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2024-04-11 15:12:22</t>
+          <t>2024-04-11 16:07:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2024-04-11 16:08:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2024-04-11 16:08:45</t>
         </is>
       </c>
     </row>

</xml_diff>